<commit_message>
Added data from quick et. al 2020
</commit_message>
<xml_diff>
--- a/data/labels/gt-bands.xlsx
+++ b/data/labels/gt-bands.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ando/Projects/sand/py-sand-mapping/data/labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEDAB66D-0611-0D44-9331-4ABA54D703EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0ED06B-D6F2-4E4D-9B1F-741E9501E54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sedinet" sheetId="1" r:id="rId1"/>
     <sheet name="mozambique" sheetId="2" r:id="rId2"/>
+    <sheet name="quick" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="469">
   <si>
     <t>ID</t>
   </si>
@@ -1267,19 +1267,186 @@
   </si>
   <si>
     <t>License 8348C Applied (2016-09-61)</t>
+  </si>
+  <si>
+    <t>Notes on how these were chosen</t>
+  </si>
+  <si>
+    <t>quick-0</t>
+  </si>
+  <si>
+    <t>gravel</t>
+  </si>
+  <si>
+    <t>2020-05-31</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.1</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Mohand river</t>
+  </si>
+  <si>
+    <t>Within Siwalik conglomerate ~10 km upstream of MFT</t>
+  </si>
+  <si>
+    <t>quick-1</t>
+  </si>
+  <si>
+    <t>2021-12-07</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.2</t>
+  </si>
+  <si>
+    <t>Within Siwalik conglomerate ~7 km upstream of MFT</t>
+  </si>
+  <si>
+    <t>quick-2</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.3</t>
+  </si>
+  <si>
+    <t>Within Middle Siwalik sandstone ~3 km upstream of MFT</t>
+  </si>
+  <si>
+    <t>quick-3</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.4</t>
+  </si>
+  <si>
+    <t>Mountain front (MFT) Near Mohand town</t>
+  </si>
+  <si>
+    <t>quick-4</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.5</t>
+  </si>
+  <si>
+    <t>~5 km downstream of MFT</t>
+  </si>
+  <si>
+    <t>quick-5</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.6</t>
+  </si>
+  <si>
+    <t>~10 downstream of MFT</t>
+  </si>
+  <si>
+    <t>quick-6</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.7</t>
+  </si>
+  <si>
+    <t>~13 km downstream of MFT</t>
+  </si>
+  <si>
+    <t>quick-7</t>
+  </si>
+  <si>
+    <t>2021-02-10</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.8</t>
+  </si>
+  <si>
+    <t>quick-8</t>
+  </si>
+  <si>
+    <t>2020-12-05</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.9</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Karnali river</t>
+  </si>
+  <si>
+    <t>~15 km downstream of MFT</t>
+  </si>
+  <si>
+    <t>quick-9</t>
+  </si>
+  <si>
+    <t>2021-01-06</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.10</t>
+  </si>
+  <si>
+    <t>~28 km downstream of MFT</t>
+  </si>
+  <si>
+    <t>quick-10</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.11</t>
+  </si>
+  <si>
+    <t>Sattighat bridge ~34 km downstream of MFT</t>
+  </si>
+  <si>
+    <t>quick-11</t>
+  </si>
+  <si>
+    <t>2020-12-23</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.12</t>
+  </si>
+  <si>
+    <t>Kosi river</t>
+  </si>
+  <si>
+    <t>~10 km downstream of MFT</t>
+  </si>
+  <si>
+    <t>quick-12</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.13</t>
+  </si>
+  <si>
+    <t>~12 km downstream of MFT,   Patchy gravel bar/ sand bar</t>
+  </si>
+  <si>
+    <t>quick-13</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1130/B35334.14</t>
+  </si>
+  <si>
+    <t>~15 km downstream of MFT,   Patchy gravel bar/ sand bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -1295,7 +1462,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1318,13 +1485,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1631,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="P86" sqref="P86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11083,7 +11268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -11628,4 +11813,1102 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Y15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B2">
+        <v>30.234560999999999</v>
+      </c>
+      <c r="C2">
+        <v>77.949155000000005</v>
+      </c>
+      <c r="D2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E2" t="s">
+        <v>418</v>
+      </c>
+      <c r="F2" t="s">
+        <v>399</v>
+      </c>
+      <c r="G2" t="s">
+        <v>419</v>
+      </c>
+      <c r="H2" t="s">
+        <v>420</v>
+      </c>
+      <c r="I2" t="s">
+        <v>421</v>
+      </c>
+      <c r="J2" t="s">
+        <v>422</v>
+      </c>
+      <c r="K2">
+        <v>1319.21240234375</v>
+      </c>
+      <c r="L2">
+        <v>1772.513305664062</v>
+      </c>
+      <c r="M2">
+        <v>2022.725708007812</v>
+      </c>
+      <c r="N2">
+        <v>2752.63720703125</v>
+      </c>
+      <c r="O2">
+        <v>2874.460205078125</v>
+      </c>
+      <c r="P2">
+        <v>3267.5751953125</v>
+      </c>
+      <c r="Q2">
+        <v>2622.114990234375</v>
+      </c>
+      <c r="R2">
+        <v>-9.3276700973510742</v>
+      </c>
+      <c r="S2">
+        <v>-16.4047737121582</v>
+      </c>
+      <c r="T2">
+        <v>5.4480250924825668E-2</v>
+      </c>
+      <c r="U2">
+        <v>0.13022275269031519</v>
+      </c>
+      <c r="V2">
+        <v>-0.2187332212924957</v>
+      </c>
+      <c r="W2" t="b">
+        <v>1</v>
+      </c>
+      <c r="X2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B3">
+        <v>30.221257999999999</v>
+      </c>
+      <c r="C3">
+        <v>77.938005000000004</v>
+      </c>
+      <c r="D3" t="s">
+        <v>417</v>
+      </c>
+      <c r="E3" t="s">
+        <v>424</v>
+      </c>
+      <c r="F3" t="s">
+        <v>399</v>
+      </c>
+      <c r="G3" t="s">
+        <v>425</v>
+      </c>
+      <c r="H3" t="s">
+        <v>420</v>
+      </c>
+      <c r="I3" t="s">
+        <v>421</v>
+      </c>
+      <c r="J3" t="s">
+        <v>426</v>
+      </c>
+      <c r="K3">
+        <v>1395.654174804688</v>
+      </c>
+      <c r="L3">
+        <v>1758.58642578125</v>
+      </c>
+      <c r="M3">
+        <v>1999.6240234375</v>
+      </c>
+      <c r="N3">
+        <v>2368.3759765625</v>
+      </c>
+      <c r="O3">
+        <v>2344.75927734375</v>
+      </c>
+      <c r="P3">
+        <v>2825.93994140625</v>
+      </c>
+      <c r="Q3">
+        <v>2527.66162109375</v>
+      </c>
+      <c r="R3">
+        <v>-9.9792757034301758</v>
+      </c>
+      <c r="S3">
+        <v>-17.18000602722168</v>
+      </c>
+      <c r="T3">
+        <v>7.5659178197383881E-2</v>
+      </c>
+      <c r="U3">
+        <v>0.1234905570745468</v>
+      </c>
+      <c r="V3">
+        <v>-0.14896683394908911</v>
+      </c>
+      <c r="W3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4">
+        <v>30.195489999999999</v>
+      </c>
+      <c r="C4">
+        <v>77.913587000000007</v>
+      </c>
+      <c r="D4" t="s">
+        <v>417</v>
+      </c>
+      <c r="E4" t="s">
+        <v>424</v>
+      </c>
+      <c r="F4" t="s">
+        <v>399</v>
+      </c>
+      <c r="G4" t="s">
+        <v>428</v>
+      </c>
+      <c r="H4" t="s">
+        <v>420</v>
+      </c>
+      <c r="I4" t="s">
+        <v>421</v>
+      </c>
+      <c r="J4" t="s">
+        <v>429</v>
+      </c>
+      <c r="K4">
+        <v>1225.929443359375</v>
+      </c>
+      <c r="L4">
+        <v>1539.88232421875</v>
+      </c>
+      <c r="M4">
+        <v>1697.811767578125</v>
+      </c>
+      <c r="N4">
+        <v>2112.411865234375</v>
+      </c>
+      <c r="O4">
+        <v>2085.01171875</v>
+      </c>
+      <c r="P4">
+        <v>2240.576416015625</v>
+      </c>
+      <c r="Q4">
+        <v>1947.035278320312</v>
+      </c>
+      <c r="R4">
+        <v>-11.31619167327881</v>
+      </c>
+      <c r="S4">
+        <v>-20.207893371582031</v>
+      </c>
+      <c r="T4">
+        <v>3.472425788640976E-2</v>
+      </c>
+      <c r="U4">
+        <v>8.2182876765727997E-2</v>
+      </c>
+      <c r="V4">
+        <v>-0.15909168124198911</v>
+      </c>
+      <c r="W4" t="b">
+        <v>1</v>
+      </c>
+      <c r="X4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>430</v>
+      </c>
+      <c r="B5">
+        <v>30.175599999999999</v>
+      </c>
+      <c r="C5">
+        <v>77.902491999999995</v>
+      </c>
+      <c r="D5" t="s">
+        <v>417</v>
+      </c>
+      <c r="E5" t="s">
+        <v>424</v>
+      </c>
+      <c r="F5" t="s">
+        <v>399</v>
+      </c>
+      <c r="G5" t="s">
+        <v>431</v>
+      </c>
+      <c r="H5" t="s">
+        <v>420</v>
+      </c>
+      <c r="I5" t="s">
+        <v>421</v>
+      </c>
+      <c r="J5" t="s">
+        <v>432</v>
+      </c>
+      <c r="K5">
+        <v>1862.130981445312</v>
+      </c>
+      <c r="L5">
+        <v>2278.583251953125</v>
+      </c>
+      <c r="M5">
+        <v>2556.666748046875</v>
+      </c>
+      <c r="N5">
+        <v>2903.41064453125</v>
+      </c>
+      <c r="O5">
+        <v>2889.72607421875</v>
+      </c>
+      <c r="P5">
+        <v>3491.96435546875</v>
+      </c>
+      <c r="Q5">
+        <v>3354.27978515625</v>
+      </c>
+      <c r="R5">
+        <v>-11.42076587677002</v>
+      </c>
+      <c r="S5">
+        <v>-19.89841270446777</v>
+      </c>
+      <c r="T5">
+        <v>8.8432244956493378E-2</v>
+      </c>
+      <c r="U5">
+        <v>0.1187233999371529</v>
+      </c>
+      <c r="V5">
+        <v>-0.1205744370818138</v>
+      </c>
+      <c r="W5" t="b">
+        <v>1</v>
+      </c>
+      <c r="X5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B6">
+        <v>30.141309</v>
+      </c>
+      <c r="C6">
+        <v>77.876064</v>
+      </c>
+      <c r="D6" t="s">
+        <v>417</v>
+      </c>
+      <c r="E6" t="s">
+        <v>424</v>
+      </c>
+      <c r="F6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G6" t="s">
+        <v>434</v>
+      </c>
+      <c r="H6" t="s">
+        <v>420</v>
+      </c>
+      <c r="I6" t="s">
+        <v>421</v>
+      </c>
+      <c r="J6" t="s">
+        <v>435</v>
+      </c>
+      <c r="K6">
+        <v>1679.537841796875</v>
+      </c>
+      <c r="L6">
+        <v>2110.77294921875</v>
+      </c>
+      <c r="M6">
+        <v>2393.282958984375</v>
+      </c>
+      <c r="N6">
+        <v>2846.816650390625</v>
+      </c>
+      <c r="O6">
+        <v>2739.498046875</v>
+      </c>
+      <c r="P6">
+        <v>3319.665283203125</v>
+      </c>
+      <c r="Q6">
+        <v>3071.0517578125</v>
+      </c>
+      <c r="R6">
+        <v>-10.85787773132324</v>
+      </c>
+      <c r="S6">
+        <v>-19.040533065795898</v>
+      </c>
+      <c r="T6">
+        <v>7.7406354248523712E-2</v>
+      </c>
+      <c r="U6">
+        <v>0.11597089469432829</v>
+      </c>
+      <c r="V6">
+        <v>-0.14894191920757291</v>
+      </c>
+      <c r="W6" t="b">
+        <v>1</v>
+      </c>
+      <c r="X6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>436</v>
+      </c>
+      <c r="B7">
+        <v>30.105671999999998</v>
+      </c>
+      <c r="C7">
+        <v>77.863433999999998</v>
+      </c>
+      <c r="D7" t="s">
+        <v>417</v>
+      </c>
+      <c r="E7" t="s">
+        <v>424</v>
+      </c>
+      <c r="F7" t="s">
+        <v>399</v>
+      </c>
+      <c r="G7" t="s">
+        <v>437</v>
+      </c>
+      <c r="H7" t="s">
+        <v>420</v>
+      </c>
+      <c r="I7" t="s">
+        <v>421</v>
+      </c>
+      <c r="J7" t="s">
+        <v>438</v>
+      </c>
+      <c r="K7">
+        <v>1115.895751953125</v>
+      </c>
+      <c r="L7">
+        <v>1459.464477539062</v>
+      </c>
+      <c r="M7">
+        <v>1710.293823242188</v>
+      </c>
+      <c r="N7">
+        <v>2459.009521484375</v>
+      </c>
+      <c r="O7">
+        <v>2430.459716796875</v>
+      </c>
+      <c r="P7">
+        <v>3117.1611328125</v>
+      </c>
+      <c r="Q7">
+        <v>2777.829345703125</v>
+      </c>
+      <c r="R7">
+        <v>-12.446267127990721</v>
+      </c>
+      <c r="S7">
+        <v>-19.905715942382809</v>
+      </c>
+      <c r="T7">
+        <v>9.5990642905235291E-2</v>
+      </c>
+      <c r="U7">
+        <v>0.15025535225868231</v>
+      </c>
+      <c r="V7">
+        <v>-0.25856742262840271</v>
+      </c>
+      <c r="W7" t="b">
+        <v>1</v>
+      </c>
+      <c r="X7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B8">
+        <v>30.085487000000001</v>
+      </c>
+      <c r="C8">
+        <v>77.848254999999995</v>
+      </c>
+      <c r="D8" t="s">
+        <v>417</v>
+      </c>
+      <c r="E8" t="s">
+        <v>424</v>
+      </c>
+      <c r="F8" t="s">
+        <v>399</v>
+      </c>
+      <c r="G8" t="s">
+        <v>440</v>
+      </c>
+      <c r="H8" t="s">
+        <v>420</v>
+      </c>
+      <c r="I8" t="s">
+        <v>421</v>
+      </c>
+      <c r="J8" t="s">
+        <v>441</v>
+      </c>
+      <c r="K8">
+        <v>1645.226440429688</v>
+      </c>
+      <c r="L8">
+        <v>2127.23583984375</v>
+      </c>
+      <c r="M8">
+        <v>2435.5849609375</v>
+      </c>
+      <c r="N8">
+        <v>2999.447998046875</v>
+      </c>
+      <c r="O8">
+        <v>2916.09912109375</v>
+      </c>
+      <c r="P8">
+        <v>3652.3349609375</v>
+      </c>
+      <c r="Q8">
+        <v>3640.231201171875</v>
+      </c>
+      <c r="R8">
+        <v>-14.024118423461911</v>
+      </c>
+      <c r="S8">
+        <v>-23.543218612670898</v>
+      </c>
+      <c r="T8">
+        <v>0.11130268126726151</v>
+      </c>
+      <c r="U8">
+        <v>0.13443812727928159</v>
+      </c>
+      <c r="V8">
+        <v>-0.17057010531425479</v>
+      </c>
+      <c r="W8" t="b">
+        <v>1</v>
+      </c>
+      <c r="X8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>442</v>
+      </c>
+      <c r="B9">
+        <v>30.234482</v>
+      </c>
+      <c r="C9">
+        <v>77.948796000000002</v>
+      </c>
+      <c r="D9" t="s">
+        <v>417</v>
+      </c>
+      <c r="E9" t="s">
+        <v>443</v>
+      </c>
+      <c r="F9" t="s">
+        <v>399</v>
+      </c>
+      <c r="G9" t="s">
+        <v>444</v>
+      </c>
+      <c r="H9" t="s">
+        <v>420</v>
+      </c>
+      <c r="I9" t="s">
+        <v>421</v>
+      </c>
+      <c r="J9" t="s">
+        <v>422</v>
+      </c>
+      <c r="W9" t="b">
+        <v>0</v>
+      </c>
+      <c r="X9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>445</v>
+      </c>
+      <c r="B10">
+        <v>28.544181999999999</v>
+      </c>
+      <c r="C10">
+        <v>81.184910000000002</v>
+      </c>
+      <c r="D10" t="s">
+        <v>417</v>
+      </c>
+      <c r="E10" t="s">
+        <v>446</v>
+      </c>
+      <c r="F10" t="s">
+        <v>399</v>
+      </c>
+      <c r="G10" t="s">
+        <v>447</v>
+      </c>
+      <c r="H10" t="s">
+        <v>448</v>
+      </c>
+      <c r="I10" t="s">
+        <v>449</v>
+      </c>
+      <c r="J10" t="s">
+        <v>450</v>
+      </c>
+      <c r="K10">
+        <v>1974.97216796875</v>
+      </c>
+      <c r="L10">
+        <v>2411.72216796875</v>
+      </c>
+      <c r="M10">
+        <v>2661.861083984375</v>
+      </c>
+      <c r="N10">
+        <v>3028.291748046875</v>
+      </c>
+      <c r="O10">
+        <v>3047.8193359375</v>
+      </c>
+      <c r="P10">
+        <v>3852.0556640625</v>
+      </c>
+      <c r="Q10">
+        <v>3733.15283203125</v>
+      </c>
+      <c r="R10">
+        <v>-14.329891204833981</v>
+      </c>
+      <c r="S10">
+        <v>-22.0659065246582</v>
+      </c>
+      <c r="T10">
+        <v>0.10082355141639709</v>
+      </c>
+      <c r="U10">
+        <v>0.13127520680427551</v>
+      </c>
+      <c r="V10">
+        <v>-0.1135201379656792</v>
+      </c>
+      <c r="W10" t="b">
+        <v>1</v>
+      </c>
+      <c r="X10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>451</v>
+      </c>
+      <c r="B11">
+        <v>28.462824000000001</v>
+      </c>
+      <c r="C11">
+        <v>81.108812</v>
+      </c>
+      <c r="D11" t="s">
+        <v>417</v>
+      </c>
+      <c r="E11" t="s">
+        <v>452</v>
+      </c>
+      <c r="F11" t="s">
+        <v>399</v>
+      </c>
+      <c r="G11" t="s">
+        <v>453</v>
+      </c>
+      <c r="H11" t="s">
+        <v>448</v>
+      </c>
+      <c r="I11" t="s">
+        <v>449</v>
+      </c>
+      <c r="J11" t="s">
+        <v>454</v>
+      </c>
+      <c r="K11">
+        <v>1985.542236328125</v>
+      </c>
+      <c r="L11">
+        <v>2329.4228515625</v>
+      </c>
+      <c r="M11">
+        <v>2542.54736328125</v>
+      </c>
+      <c r="N11">
+        <v>2934.612060546875</v>
+      </c>
+      <c r="O11">
+        <v>2910.124267578125</v>
+      </c>
+      <c r="P11">
+        <v>3800.383056640625</v>
+      </c>
+      <c r="Q11">
+        <v>3829.13427734375</v>
+      </c>
+      <c r="R11">
+        <v>-16.072820663452148</v>
+      </c>
+      <c r="S11">
+        <v>-25.77334022521973</v>
+      </c>
+      <c r="T11">
+        <v>0.1066755428910255</v>
+      </c>
+      <c r="U11">
+        <v>0.12663425505161291</v>
+      </c>
+      <c r="V11">
+        <v>-0.1151818484067917</v>
+      </c>
+      <c r="W11" t="b">
+        <v>1</v>
+      </c>
+      <c r="X11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>455</v>
+      </c>
+      <c r="B12">
+        <v>28.427043999999999</v>
+      </c>
+      <c r="C12">
+        <v>81.071270999999996</v>
+      </c>
+      <c r="D12" t="s">
+        <v>417</v>
+      </c>
+      <c r="E12" t="s">
+        <v>452</v>
+      </c>
+      <c r="F12" t="s">
+        <v>399</v>
+      </c>
+      <c r="G12" t="s">
+        <v>456</v>
+      </c>
+      <c r="H12" t="s">
+        <v>448</v>
+      </c>
+      <c r="I12" t="s">
+        <v>449</v>
+      </c>
+      <c r="J12" t="s">
+        <v>457</v>
+      </c>
+      <c r="K12">
+        <v>1786.4560546875</v>
+      </c>
+      <c r="L12">
+        <v>2092.47705078125</v>
+      </c>
+      <c r="M12">
+        <v>2266.569091796875</v>
+      </c>
+      <c r="N12">
+        <v>2521.385009765625</v>
+      </c>
+      <c r="O12">
+        <v>2467.58984375</v>
+      </c>
+      <c r="P12">
+        <v>3157.702880859375</v>
+      </c>
+      <c r="Q12">
+        <v>3161.217529296875</v>
+      </c>
+      <c r="R12">
+        <v>-11.78465747833252</v>
+      </c>
+      <c r="S12">
+        <v>-19.811862945556641</v>
+      </c>
+      <c r="T12">
+        <v>9.445490688085556E-2</v>
+      </c>
+      <c r="U12">
+        <v>0.1143985316157341</v>
+      </c>
+      <c r="V12">
+        <v>-9.2429518699645996E-2</v>
+      </c>
+      <c r="W12" t="b">
+        <v>1</v>
+      </c>
+      <c r="X12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>458</v>
+      </c>
+      <c r="B13">
+        <v>26.774809000000001</v>
+      </c>
+      <c r="C13">
+        <v>87.126765000000006</v>
+      </c>
+      <c r="D13" t="s">
+        <v>417</v>
+      </c>
+      <c r="E13" t="s">
+        <v>459</v>
+      </c>
+      <c r="F13" t="s">
+        <v>399</v>
+      </c>
+      <c r="G13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H13" t="s">
+        <v>448</v>
+      </c>
+      <c r="I13" t="s">
+        <v>461</v>
+      </c>
+      <c r="J13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K13">
+        <v>2175.842041015625</v>
+      </c>
+      <c r="L13">
+        <v>2481.21044921875</v>
+      </c>
+      <c r="M13">
+        <v>2678.394775390625</v>
+      </c>
+      <c r="N13">
+        <v>2822.671142578125</v>
+      </c>
+      <c r="O13">
+        <v>2787.868408203125</v>
+      </c>
+      <c r="P13">
+        <v>3680.618408203125</v>
+      </c>
+      <c r="Q13">
+        <v>3993.0263671875</v>
+      </c>
+      <c r="R13">
+        <v>-14.96737670898438</v>
+      </c>
+      <c r="S13">
+        <v>-25.43132209777832</v>
+      </c>
+      <c r="T13">
+        <v>0.1182191371917725</v>
+      </c>
+      <c r="U13">
+        <v>0.1198164001107216</v>
+      </c>
+      <c r="V13">
+        <v>-6.4419254660606384E-2</v>
+      </c>
+      <c r="W13" t="b">
+        <v>1</v>
+      </c>
+      <c r="X13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>463</v>
+      </c>
+      <c r="B14">
+        <v>26.753926</v>
+      </c>
+      <c r="C14">
+        <v>87.116090999999997</v>
+      </c>
+      <c r="D14" t="s">
+        <v>417</v>
+      </c>
+      <c r="E14" t="s">
+        <v>459</v>
+      </c>
+      <c r="F14" t="s">
+        <v>399</v>
+      </c>
+      <c r="G14" t="s">
+        <v>464</v>
+      </c>
+      <c r="H14" t="s">
+        <v>448</v>
+      </c>
+      <c r="I14" t="s">
+        <v>461</v>
+      </c>
+      <c r="J14" t="s">
+        <v>465</v>
+      </c>
+      <c r="K14">
+        <v>2123.6240234375</v>
+      </c>
+      <c r="L14">
+        <v>2415.278076171875</v>
+      </c>
+      <c r="M14">
+        <v>2605.082763671875</v>
+      </c>
+      <c r="N14">
+        <v>2727.96240234375</v>
+      </c>
+      <c r="O14">
+        <v>2719.954833984375</v>
+      </c>
+      <c r="P14">
+        <v>3724.804443359375</v>
+      </c>
+      <c r="Q14">
+        <v>4098.91748046875</v>
+      </c>
+      <c r="R14">
+        <v>-18.23663330078125</v>
+      </c>
+      <c r="S14">
+        <v>-26.507944107055661</v>
+      </c>
+      <c r="T14">
+        <v>0.13260059058666229</v>
+      </c>
+      <c r="U14">
+        <v>0.13221900165081019</v>
+      </c>
+      <c r="V14">
+        <v>-6.0791332274675369E-2</v>
+      </c>
+      <c r="W14" t="b">
+        <v>1</v>
+      </c>
+      <c r="X14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>466</v>
+      </c>
+      <c r="B15">
+        <v>26.726535999999999</v>
+      </c>
+      <c r="C15">
+        <v>87.108413999999996</v>
+      </c>
+      <c r="D15" t="s">
+        <v>417</v>
+      </c>
+      <c r="E15" t="s">
+        <v>459</v>
+      </c>
+      <c r="F15" t="s">
+        <v>399</v>
+      </c>
+      <c r="G15" t="s">
+        <v>467</v>
+      </c>
+      <c r="H15" t="s">
+        <v>448</v>
+      </c>
+      <c r="I15" t="s">
+        <v>461</v>
+      </c>
+      <c r="J15" t="s">
+        <v>468</v>
+      </c>
+      <c r="W15" t="b">
+        <v>0</v>
+      </c>
+      <c r="X15" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated training dataset with results from Dingle et al 2016
</commit_message>
<xml_diff>
--- a/data/labels/gt-bands.xlsx
+++ b/data/labels/gt-bands.xlsx
@@ -10,6 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mozambique" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="quick" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dingle2020" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dingle2016" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -14215,4 +14216,2003 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Latitude</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Longitude</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Site</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>Distance Downstram of MFT (km)</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>D84</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>D50</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>B2_mean</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>B3_mean</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>B4_mean</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
+        <is>
+          <t>B8_mean</t>
+        </is>
+      </c>
+      <c r="Q1" s="3" t="inlineStr">
+        <is>
+          <t>B8A_mean</t>
+        </is>
+      </c>
+      <c r="R1" s="3" t="inlineStr">
+        <is>
+          <t>B11_mean</t>
+        </is>
+      </c>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>B12_mean</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
+        <is>
+          <t>VV_mean</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>VH_mean</t>
+        </is>
+      </c>
+      <c r="V1" s="3" t="inlineStr">
+        <is>
+          <t>mTGSI_mean</t>
+        </is>
+      </c>
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>BSI_mean</t>
+        </is>
+      </c>
+      <c r="X1" s="3" t="inlineStr">
+        <is>
+          <t>NDWI_mean</t>
+        </is>
+      </c>
+      <c r="Y1" s="3" t="inlineStr">
+        <is>
+          <t>keep</t>
+        </is>
+      </c>
+      <c r="Z1" s="3" t="inlineStr">
+        <is>
+          <t>location_tweaked</t>
+        </is>
+      </c>
+      <c r="AA1" s="3" t="inlineStr">
+        <is>
+          <t>class_code</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>dingle16-yamuna-0</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>30.29146</v>
+      </c>
+      <c r="C2" t="n">
+        <v>77.561964</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.03</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Yamuna</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>109.896376</v>
+      </c>
+      <c r="L2" t="n">
+        <v>60.5476894</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1347.421264648438</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1602.337036132812</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1739.076904296875</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2041.135498046875</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1950.637329101562</v>
+      </c>
+      <c r="R2" t="n">
+        <v>2219.377197265625</v>
+      </c>
+      <c r="S2" t="n">
+        <v>2056.53125</v>
+      </c>
+      <c r="T2" t="n">
+        <v>-9.634684562683105</v>
+      </c>
+      <c r="U2" t="n">
+        <v>-18.92320251464844</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.04677057638764381</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.07787266373634338</v>
+      </c>
+      <c r="X2" t="n">
+        <v>-0.1212015524506569</v>
+      </c>
+      <c r="Y2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>dingle16-yamuna-1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>30.260467</v>
+      </c>
+      <c r="C3" t="n">
+        <v>77.531451</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.04</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Yamuna</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="K3" t="n">
+        <v>167.730356</v>
+      </c>
+      <c r="L3" t="n">
+        <v>87.4265764</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1543.453491210938</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1877.674438476562</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2071.267333984375</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2345.104736328125</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2242.156982421875</v>
+      </c>
+      <c r="R3" t="n">
+        <v>2543.482666015625</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2409.145263671875</v>
+      </c>
+      <c r="T3" t="n">
+        <v>-11.07124328613281</v>
+      </c>
+      <c r="U3" t="n">
+        <v>-21.28955268859863</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.05740170925855637</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.08444039523601532</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-0.1103412136435509</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>dingle16-yamuna-2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>30.169525</v>
+      </c>
+      <c r="C4" t="n">
+        <v>77.476584</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.05</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Yamuna</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>79.34129280000001</v>
+      </c>
+      <c r="L4" t="n">
+        <v>37.7917652</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1256.974853515625</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1516.1005859375</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1689.848999023438</v>
+      </c>
+      <c r="P4" t="n">
+        <v>2091.660400390625</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2051.53466796875</v>
+      </c>
+      <c r="R4" t="n">
+        <v>2373.446533203125</v>
+      </c>
+      <c r="S4" t="n">
+        <v>2117.2705078125</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-10.77158164978027</v>
+      </c>
+      <c r="U4" t="n">
+        <v>-18.29835319519043</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.05307880416512489</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.09663672000169754</v>
+      </c>
+      <c r="X4" t="n">
+        <v>-0.1617854833602905</v>
+      </c>
+      <c r="Y4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>dingle16-yamuna-3</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>30.148757</v>
+      </c>
+      <c r="C5" t="n">
+        <v>77.45776499999999</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2022-02-14</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.06</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Yamuna</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>32</v>
+      </c>
+      <c r="K5" t="n">
+        <v>68.1196917</v>
+      </c>
+      <c r="L5" t="n">
+        <v>33.8245773</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1544.547729492188</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1814.71337890625</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1971.184692382812</v>
+      </c>
+      <c r="P5" t="n">
+        <v>2210.8916015625</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2137.39501953125</v>
+      </c>
+      <c r="R5" t="n">
+        <v>2491.1083984375</v>
+      </c>
+      <c r="S5" t="n">
+        <v>2440.038330078125</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-10.74287605285645</v>
+      </c>
+      <c r="U5" t="n">
+        <v>-19.26670074462891</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.06509967893362045</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.08539595454931259</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-0.09833177924156189</v>
+      </c>
+      <c r="Y5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>dingle16-ganga-0</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>30.050727</v>
+      </c>
+      <c r="C6" t="n">
+        <v>78.272932</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2022-11-15</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.07</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Ganga</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>-4.3</v>
+      </c>
+      <c r="K6" t="n">
+        <v>215.269482</v>
+      </c>
+      <c r="L6" t="n">
+        <v>89.884472</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2465.386474609375</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2744.988525390625</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2952.647705078125</v>
+      </c>
+      <c r="P6" t="n">
+        <v>3069.852294921875</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>3078.3408203125</v>
+      </c>
+      <c r="R6" t="n">
+        <v>3622.755615234375</v>
+      </c>
+      <c r="S6" t="n">
+        <v>3593.54541015625</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-11.00167846679688</v>
+      </c>
+      <c r="U6" t="n">
+        <v>-18.94388580322266</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.06821431964635849</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.08592848479747772</v>
+      </c>
+      <c r="X6" t="n">
+        <v>-0.05591895058751106</v>
+      </c>
+      <c r="Y6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>dingle16-ganga-1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>29.906995</v>
+      </c>
+      <c r="C7" t="n">
+        <v>78.163685</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2022-11-15</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.08</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Ganga</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="K7" t="n">
+        <v>176.069353</v>
+      </c>
+      <c r="L7" t="n">
+        <v>109.896376</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2270.199951171875</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2618.239990234375</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2862.860107421875</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3079.090087890625</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>3129.239990234375</v>
+      </c>
+      <c r="R7" t="n">
+        <v>3604.64990234375</v>
+      </c>
+      <c r="S7" t="n">
+        <v>3512.469970703125</v>
+      </c>
+      <c r="T7" t="n">
+        <v>-10.80661773681641</v>
+      </c>
+      <c r="U7" t="n">
+        <v>-19.3923168182373</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.07100006937980652</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.09478229284286499</v>
+      </c>
+      <c r="X7" t="n">
+        <v>-0.08251048624515533</v>
+      </c>
+      <c r="Y7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>dingle16-ganga-2</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>29.8788894</v>
+      </c>
+      <c r="C8" t="n">
+        <v>78.17294080000001</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2022-11-15</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.09</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Ganga</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>11.7</v>
+      </c>
+      <c r="K8" t="n">
+        <v>149.085899</v>
+      </c>
+      <c r="L8" t="n">
+        <v>97.00586029999999</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1208.391357421875</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1486</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1651.076049804688</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2030.054321289062</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>2040.978271484375</v>
+      </c>
+      <c r="R8" t="n">
+        <v>2465.141357421875</v>
+      </c>
+      <c r="S8" t="n">
+        <v>2261.391357421875</v>
+      </c>
+      <c r="T8" t="n">
+        <v>-7.834619045257568</v>
+      </c>
+      <c r="U8" t="n">
+        <v>-16.4534969329834</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.07813765108585358</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.1202901676297188</v>
+      </c>
+      <c r="X8" t="n">
+        <v>-0.1554068773984909</v>
+      </c>
+      <c r="Y8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>dingle16-ganga-3</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>29.792369</v>
+      </c>
+      <c r="C9" t="n">
+        <v>78.173349</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2022-11-15</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.10</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Ganga</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>22.1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>76.6386371</v>
+      </c>
+      <c r="L9" t="n">
+        <v>37.7917652</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1983.168823242188</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2347.818115234375</v>
+      </c>
+      <c r="O9" t="n">
+        <v>2600.571533203125</v>
+      </c>
+      <c r="P9" t="n">
+        <v>2845.3896484375</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>2886.532470703125</v>
+      </c>
+      <c r="R9" t="n">
+        <v>3489.3701171875</v>
+      </c>
+      <c r="S9" t="n">
+        <v>3545.863525390625</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-8.71595287322998</v>
+      </c>
+      <c r="U9" t="n">
+        <v>-17.02326202392578</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.09884721785783768</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.1155252754688263</v>
+      </c>
+      <c r="X9" t="n">
+        <v>-0.09567610919475555</v>
+      </c>
+      <c r="Y9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>dingle16-sharda-0</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>29.1022936</v>
+      </c>
+      <c r="C10" t="n">
+        <v>80.14201420000001</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2022-05-13</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.11</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Sharda</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>306.554548</v>
+      </c>
+      <c r="L10" t="n">
+        <v>83.8651778</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1934.971923828125</v>
+      </c>
+      <c r="N10" t="n">
+        <v>2264.5419921875</v>
+      </c>
+      <c r="O10" t="n">
+        <v>2466.915771484375</v>
+      </c>
+      <c r="P10" t="n">
+        <v>2600.99072265625</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>2566.897216796875</v>
+      </c>
+      <c r="R10" t="n">
+        <v>3207.373779296875</v>
+      </c>
+      <c r="S10" t="n">
+        <v>3220.383056640625</v>
+      </c>
+      <c r="T10" t="n">
+        <v>-13.89581871032715</v>
+      </c>
+      <c r="U10" t="n">
+        <v>-25.60627174377441</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.09235741198062897</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.1117485910654068</v>
+      </c>
+      <c r="X10" t="n">
+        <v>-0.06837564706802368</v>
+      </c>
+      <c r="Y10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>dingle16-sharda-1</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>29.075778</v>
+      </c>
+      <c r="C11" t="n">
+        <v>80.123819</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2022-05-13</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.12</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Sharda</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="K11" t="n">
+        <v>69.5510312</v>
+      </c>
+      <c r="L11" t="n">
+        <v>24.7610399</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1823.0234375</v>
+      </c>
+      <c r="N11" t="n">
+        <v>2056.8125</v>
+      </c>
+      <c r="O11" t="n">
+        <v>2197.78125</v>
+      </c>
+      <c r="P11" t="n">
+        <v>2373.78515625</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2431.81640625</v>
+      </c>
+      <c r="R11" t="n">
+        <v>3055.79296875</v>
+      </c>
+      <c r="S11" t="n">
+        <v>3083.984375</v>
+      </c>
+      <c r="T11" t="n">
+        <v>-14.74081230163574</v>
+      </c>
+      <c r="U11" t="n">
+        <v>-25.13649749755859</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.09337495267391205</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.1112270951271057</v>
+      </c>
+      <c r="X11" t="n">
+        <v>-0.07106124609708786</v>
+      </c>
+      <c r="Y11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>dingle16-sharda-2</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>29.020309</v>
+      </c>
+      <c r="C12" t="n">
+        <v>80.09943199999999</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2022-05-13</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.13</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Sharda</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="K12" t="n">
+        <v>195.361179</v>
+      </c>
+      <c r="L12" t="n">
+        <v>96.3357918</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1929.218139648438</v>
+      </c>
+      <c r="N12" t="n">
+        <v>2217.63037109375</v>
+      </c>
+      <c r="O12" t="n">
+        <v>2391.375732421875</v>
+      </c>
+      <c r="P12" t="n">
+        <v>2645.833251953125</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>2727.787841796875</v>
+      </c>
+      <c r="R12" t="n">
+        <v>3298.7939453125</v>
+      </c>
+      <c r="S12" t="n">
+        <v>3087.833251953125</v>
+      </c>
+      <c r="T12" t="n">
+        <v>-7.853887557983398</v>
+      </c>
+      <c r="U12" t="n">
+        <v>-16.9774341583252</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.07366131991147995</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.1086284145712852</v>
+      </c>
+      <c r="X12" t="n">
+        <v>-0.08803794533014297</v>
+      </c>
+      <c r="Y12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>dingle16-sharda-3</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>28.9408923</v>
+      </c>
+      <c r="C13" t="n">
+        <v>80.1127609</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2022-11-15</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.14</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Sharda</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>23.7</v>
+      </c>
+      <c r="K13" t="n">
+        <v>81.5718801</v>
+      </c>
+      <c r="L13" t="n">
+        <v>52.7098251</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1892.636840820312</v>
+      </c>
+      <c r="N13" t="n">
+        <v>2157.65185546875</v>
+      </c>
+      <c r="O13" t="n">
+        <v>2266.9453125</v>
+      </c>
+      <c r="P13" t="n">
+        <v>2421.5771484375</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>2554.905517578125</v>
+      </c>
+      <c r="R13" t="n">
+        <v>2968.109375</v>
+      </c>
+      <c r="S13" t="n">
+        <v>2827.76611328125</v>
+      </c>
+      <c r="T13" t="n">
+        <v>-16.84579086303711</v>
+      </c>
+      <c r="U13" t="n">
+        <v>-25.94126129150391</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.06690531224012375</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.09633225202560425</v>
+      </c>
+      <c r="X13" t="n">
+        <v>-0.05918433517217636</v>
+      </c>
+      <c r="Y13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>dingle16-sharda-4</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>28.920551</v>
+      </c>
+      <c r="C14" t="n">
+        <v>80.113148</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2022-11-15</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.15</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Sharda</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="K14" t="n">
+        <v>100.426765</v>
+      </c>
+      <c r="L14" t="n">
+        <v>54.9481879</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2033.37841796875</v>
+      </c>
+      <c r="N14" t="n">
+        <v>2354.350830078125</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2563.760009765625</v>
+      </c>
+      <c r="P14" t="n">
+        <v>2775.760009765625</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>2745.350830078125</v>
+      </c>
+      <c r="R14" t="n">
+        <v>3335.596923828125</v>
+      </c>
+      <c r="S14" t="n">
+        <v>3342.504638671875</v>
+      </c>
+      <c r="T14" t="n">
+        <v>-14.58208274841309</v>
+      </c>
+      <c r="U14" t="n">
+        <v>-23.89912033081055</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.08401543647050858</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.1019510850310326</v>
+      </c>
+      <c r="X14" t="n">
+        <v>-0.08249806612730026</v>
+      </c>
+      <c r="Y14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>dingle16-sharda-5</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>28.8147</v>
+      </c>
+      <c r="C15" t="n">
+        <v>80.11038000000001</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2022-11-15</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.16</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Sharda</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="K15" t="n">
+        <v>72.003743</v>
+      </c>
+      <c r="L15" t="n">
+        <v>46.8507423</v>
+      </c>
+      <c r="M15" t="n">
+        <v>2423.2275390625</v>
+      </c>
+      <c r="N15" t="n">
+        <v>2791.544921875</v>
+      </c>
+      <c r="O15" t="n">
+        <v>3016.413818359375</v>
+      </c>
+      <c r="P15" t="n">
+        <v>3192.034423828125</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>3135.089599609375</v>
+      </c>
+      <c r="R15" t="n">
+        <v>3585.627685546875</v>
+      </c>
+      <c r="S15" t="n">
+        <v>3541.28271484375</v>
+      </c>
+      <c r="T15" t="n">
+        <v>-15.86105346679688</v>
+      </c>
+      <c r="U15" t="n">
+        <v>-26.53816986083984</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.06319303810596466</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.08108559250831604</v>
+      </c>
+      <c r="X15" t="n">
+        <v>-0.06691616773605347</v>
+      </c>
+      <c r="Y15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>dingle16-gandak-0</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>27.4634675</v>
+      </c>
+      <c r="C16" t="n">
+        <v>83.9416274</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2018-12-11</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.17</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Gandak</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>81.5718801</v>
+      </c>
+      <c r="L16" t="n">
+        <v>82.71058119999999</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1940.073364257812</v>
+      </c>
+      <c r="N16" t="n">
+        <v>2314.12841796875</v>
+      </c>
+      <c r="O16" t="n">
+        <v>2527.5595703125</v>
+      </c>
+      <c r="P16" t="n">
+        <v>2832.1376953125</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>2772.981689453125</v>
+      </c>
+      <c r="R16" t="n">
+        <v>3452.60546875</v>
+      </c>
+      <c r="S16" t="n">
+        <v>3441.08251953125</v>
+      </c>
+      <c r="T16" t="n">
+        <v>-13.6841459274292</v>
+      </c>
+      <c r="U16" t="n">
+        <v>-21.05259323120117</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.09186574816703796</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.1126137748360634</v>
+      </c>
+      <c r="X16" t="n">
+        <v>-0.1012742966413498</v>
+      </c>
+      <c r="Y16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>dingle16-kosi-0</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>26.8436685</v>
+      </c>
+      <c r="C17" t="n">
+        <v>87.14920669999999</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2018-12-11</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.21</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Kosi</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>286.025507</v>
+      </c>
+      <c r="L17" t="n">
+        <v>85.0358921</v>
+      </c>
+      <c r="M17" t="n">
+        <v>2079.427490234375</v>
+      </c>
+      <c r="N17" t="n">
+        <v>2398.289794921875</v>
+      </c>
+      <c r="O17" t="n">
+        <v>2601.293212890625</v>
+      </c>
+      <c r="P17" t="n">
+        <v>2793.1943359375</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>2762.155517578125</v>
+      </c>
+      <c r="R17" t="n">
+        <v>3704.49462890625</v>
+      </c>
+      <c r="S17" t="n">
+        <v>3895.872802734375</v>
+      </c>
+      <c r="T17" t="n">
+        <v>-12.5465669631958</v>
+      </c>
+      <c r="U17" t="n">
+        <v>-23.32100296020508</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.1180772706866264</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.1284811794757843</v>
+      </c>
+      <c r="X17" t="n">
+        <v>-0.07635822892189026</v>
+      </c>
+      <c r="Y17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>dingle16-kosi-1</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>26.8349792</v>
+      </c>
+      <c r="C18" t="n">
+        <v>87.1439618</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2018-12-11</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.22</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Kosi</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K18" t="n">
+        <v>205.073889</v>
+      </c>
+      <c r="L18" t="n">
+        <v>111.430472</v>
+      </c>
+      <c r="M18" t="n">
+        <v>2000.145385742188</v>
+      </c>
+      <c r="N18" t="n">
+        <v>2367.907470703125</v>
+      </c>
+      <c r="O18" t="n">
+        <v>2585.911865234375</v>
+      </c>
+      <c r="P18" t="n">
+        <v>2774.713623046875</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>2742.061767578125</v>
+      </c>
+      <c r="R18" t="n">
+        <v>3513.87451171875</v>
+      </c>
+      <c r="S18" t="n">
+        <v>3639.81494140625</v>
+      </c>
+      <c r="T18" t="n">
+        <v>-11.54463386535645</v>
+      </c>
+      <c r="U18" t="n">
+        <v>-20.67917823791504</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.1083866134285927</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0.1216041967272758</v>
+      </c>
+      <c r="X18" t="n">
+        <v>-0.07910560071468353</v>
+      </c>
+      <c r="Y18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>dingle16-kosi-2</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>26.811374</v>
+      </c>
+      <c r="C19" t="n">
+        <v>87.152321</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2018-12-11</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.23</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Kosi</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>42</v>
+      </c>
+      <c r="K19" t="n">
+        <v>85.0358921</v>
+      </c>
+      <c r="L19" t="n">
+        <v>42.2242531</v>
+      </c>
+      <c r="M19" t="n">
+        <v>2192.204833984375</v>
+      </c>
+      <c r="N19" t="n">
+        <v>2572.56689453125</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2827.43310546875</v>
+      </c>
+      <c r="P19" t="n">
+        <v>3014.275634765625</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>2929.18115234375</v>
+      </c>
+      <c r="R19" t="n">
+        <v>3962</v>
+      </c>
+      <c r="S19" t="n">
+        <v>4239.80322265625</v>
+      </c>
+      <c r="T19" t="n">
+        <v>-10.55954933166504</v>
+      </c>
+      <c r="U19" t="n">
+        <v>-20.33795738220215</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.1245162039995193</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0.1312774270772934</v>
+      </c>
+      <c r="X19" t="n">
+        <v>-0.07948710769414902</v>
+      </c>
+      <c r="Y19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>dingle16-kosi-3</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>26.787227</v>
+      </c>
+      <c r="C20" t="n">
+        <v>87.12368600000001</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2018-12-11</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>10.2475/08.2016.24</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Kosi</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="K20" t="n">
+        <v>135.298309</v>
+      </c>
+      <c r="L20" t="n">
+        <v>63.5579197</v>
+      </c>
+      <c r="M20" t="n">
+        <v>2387.865478515625</v>
+      </c>
+      <c r="N20" t="n">
+        <v>2763.817138671875</v>
+      </c>
+      <c r="O20" t="n">
+        <v>2986.870849609375</v>
+      </c>
+      <c r="P20" t="n">
+        <v>3141.317138671875</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>3082.3818359375</v>
+      </c>
+      <c r="R20" t="n">
+        <v>4161.7958984375</v>
+      </c>
+      <c r="S20" t="n">
+        <v>4493.921875</v>
+      </c>
+      <c r="T20" t="n">
+        <v>-12.57971858978271</v>
+      </c>
+      <c r="U20" t="n">
+        <v>-22.9748592376709</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.1236211881041527</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0.1276864409446716</v>
+      </c>
+      <c r="X20" t="n">
+        <v>-0.06390959024429321</v>
+      </c>
+      <c r="Y20" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated nonsand and sand classes, created baseline global training and inference notebook
</commit_message>
<xml_diff>
--- a/data/labels/gt-bands.xlsx
+++ b/data/labels/gt-bands.xlsx
@@ -11,6 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="quick" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dingle2020" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dingle2016" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nonsand" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -16215,4 +16216,2017 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Latitude</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Longitude</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Site</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>B2_mean</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>B3_mean</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>B4_mean</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>B8_mean</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>B8A_mean</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>B11_mean</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
+        <is>
+          <t>B12_mean</t>
+        </is>
+      </c>
+      <c r="Q1" s="3" t="inlineStr">
+        <is>
+          <t>VV_mean</t>
+        </is>
+      </c>
+      <c r="R1" s="3" t="inlineStr">
+        <is>
+          <t>VH_mean</t>
+        </is>
+      </c>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>mTGSI_mean</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
+        <is>
+          <t>BSI_mean</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>NDWI_mean</t>
+        </is>
+      </c>
+      <c r="V1" s="3" t="inlineStr">
+        <is>
+          <t>keep</t>
+        </is>
+      </c>
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>location_tweaked</t>
+        </is>
+      </c>
+      <c r="X1" s="3" t="inlineStr">
+        <is>
+          <t>class_code</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ns-0</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>25.449886</v>
+      </c>
+      <c r="C2" t="n">
+        <v>82.858051</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>bare</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2022-10-03</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Airport</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Varanasi Airport</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>2079.636474609375</v>
+      </c>
+      <c r="K2" t="n">
+        <v>2473.57568359375</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2716.833251953125</v>
+      </c>
+      <c r="M2" t="n">
+        <v>3186.348388671875</v>
+      </c>
+      <c r="N2" t="n">
+        <v>3365.037841796875</v>
+      </c>
+      <c r="O2" t="n">
+        <v>3911.12109375</v>
+      </c>
+      <c r="P2" t="n">
+        <v>3898.12109375</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-16.30632209777832</v>
+      </c>
+      <c r="R2" t="n">
+        <v>-23.79282379150391</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.09387604892253876</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.1148049458861351</v>
+      </c>
+      <c r="U2" t="n">
+        <v>-0.1271180808544159</v>
+      </c>
+      <c r="V2" t="b">
+        <v>1</v>
+      </c>
+      <c r="W2" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ns-1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>25.230677</v>
+      </c>
+      <c r="C3" t="n">
+        <v>83.02153300000001</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>greenveg</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2020-12-11</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Vegetated Fields</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Off Ganga</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>438.1982116699219</v>
+      </c>
+      <c r="K3" t="n">
+        <v>855.1531372070312</v>
+      </c>
+      <c r="L3" t="n">
+        <v>490.5135192871094</v>
+      </c>
+      <c r="M3" t="n">
+        <v>4140.2880859375</v>
+      </c>
+      <c r="N3" t="n">
+        <v>4411</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2346.06298828125</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1156.909912109375</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-9.820938110351562</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-15.81100273132324</v>
+      </c>
+      <c r="S3" t="n">
+        <v>-0.4135011434555054</v>
+      </c>
+      <c r="T3" t="n">
+        <v>-0.2342686504125595</v>
+      </c>
+      <c r="U3" t="n">
+        <v>-0.6568585634231567</v>
+      </c>
+      <c r="V3" t="b">
+        <v>1</v>
+      </c>
+      <c r="W3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ns-2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>25.246734</v>
+      </c>
+      <c r="C4" t="n">
+        <v>83.025929</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>bare</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2022-02-19</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Bare fields</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Off Ganga</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>1274.894165039062</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1359.176513671875</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1304.282348632812</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2327.482421875</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2324.417724609375</v>
+      </c>
+      <c r="O4" t="n">
+        <v>2501.282470703125</v>
+      </c>
+      <c r="P4" t="n">
+        <v>2008.023559570312</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-13.69592094421387</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-20.93885803222656</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-0.0357835479080677</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.02703789807856083</v>
+      </c>
+      <c r="U4" t="n">
+        <v>-0.2619343400001526</v>
+      </c>
+      <c r="V4" t="b">
+        <v>1</v>
+      </c>
+      <c r="W4" t="b">
+        <v>1</v>
+      </c>
+      <c r="X4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ns-3</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>25.208222</v>
+      </c>
+      <c r="C5" t="n">
+        <v>82.980644</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2022-02-19</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>River water</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ganga</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>296.3296203613281</v>
+      </c>
+      <c r="K5" t="n">
+        <v>392.905029296875</v>
+      </c>
+      <c r="L5" t="n">
+        <v>248.6424560546875</v>
+      </c>
+      <c r="M5" t="n">
+        <v>237.1229095458984</v>
+      </c>
+      <c r="N5" t="n">
+        <v>178.2402191162109</v>
+      </c>
+      <c r="O5" t="n">
+        <v>125.6480484008789</v>
+      </c>
+      <c r="P5" t="n">
+        <v>122.2737426757812</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-25.81295585632324</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-27.55410385131836</v>
+      </c>
+      <c r="S5" t="n">
+        <v>-0.125209242105484</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-0.1751542538404465</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.2471062988042831</v>
+      </c>
+      <c r="V5" t="b">
+        <v>1</v>
+      </c>
+      <c r="W5" t="b">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ns-4</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>22.573932</v>
+      </c>
+      <c r="C6" t="n">
+        <v>88.349081</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>bare</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2022-01-02</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Urban scene, kolkata</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Off Hoogly</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>655.1570434570312</v>
+      </c>
+      <c r="K6" t="n">
+        <v>716.6033325195312</v>
+      </c>
+      <c r="L6" t="n">
+        <v>716.8099365234375</v>
+      </c>
+      <c r="M6" t="n">
+        <v>971.2975463867188</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1054.752075195312</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1108.735595703125</v>
+      </c>
+      <c r="P6" t="n">
+        <v>895.0661010742188</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-6.657454013824463</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-13.57480239868164</v>
+      </c>
+      <c r="S6" t="n">
+        <v>-0.001647719531320035</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.05957241356372833</v>
+      </c>
+      <c r="U6" t="n">
+        <v>-0.1421889066696167</v>
+      </c>
+      <c r="V6" t="b">
+        <v>1</v>
+      </c>
+      <c r="W6" t="b">
+        <v>1</v>
+      </c>
+      <c r="X6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ns-5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>22.642989</v>
+      </c>
+      <c r="C7" t="n">
+        <v>88.43940600000001</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>bare</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2020-05-11</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Airport building</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Kolkata airport</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>4966.9208984375</v>
+      </c>
+      <c r="K7" t="n">
+        <v>5988.57568359375</v>
+      </c>
+      <c r="L7" t="n">
+        <v>6438.40283203125</v>
+      </c>
+      <c r="M7" t="n">
+        <v>5973.05029296875</v>
+      </c>
+      <c r="N7" t="n">
+        <v>6263.98583984375</v>
+      </c>
+      <c r="O7" t="n">
+        <v>7159.294921875</v>
+      </c>
+      <c r="P7" t="n">
+        <v>7827.02880859375</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>7.74493408203125</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-1.827148675918579</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.1072362661361694</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.1092060059309006</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.001565491314977407</v>
+      </c>
+      <c r="V7" t="b">
+        <v>1</v>
+      </c>
+      <c r="W7" t="b">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ns-6</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>19.751838</v>
+      </c>
+      <c r="C8" t="n">
+        <v>85.702412</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>whitewater</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2021-07-11</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Off Puri</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Puri beach</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>1990.053100585938</v>
+      </c>
+      <c r="K8" t="n">
+        <v>2295.1416015625</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2225.21240234375</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1940.230102539062</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1931.800903320312</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1342.601806640625</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1110.654907226562</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-14.99519538879395</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-25.04825019836426</v>
+      </c>
+      <c r="S8" t="n">
+        <v>-0.04694213718175888</v>
+      </c>
+      <c r="T8" t="n">
+        <v>-0.02872852236032486</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.08209085464477539</v>
+      </c>
+      <c r="V8" t="b">
+        <v>1</v>
+      </c>
+      <c r="W8" t="b">
+        <v>1</v>
+      </c>
+      <c r="X8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ns-7</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>19.744671</v>
+      </c>
+      <c r="C9" t="n">
+        <v>85.694326</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2020-09-08</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Off Puri</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Puri beach</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>154.6243286132812</v>
+      </c>
+      <c r="K9" t="n">
+        <v>199.5459442138672</v>
+      </c>
+      <c r="L9" t="n">
+        <v>56.18918991088867</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.92432427406311</v>
+      </c>
+      <c r="N9" t="n">
+        <v>7.516216278076172</v>
+      </c>
+      <c r="O9" t="n">
+        <v>62.47027206420898</v>
+      </c>
+      <c r="P9" t="n">
+        <v>90.25675964355469</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-18.29485893249512</v>
+      </c>
+      <c r="R9" t="n">
+        <v>-27.12454986572266</v>
+      </c>
+      <c r="S9" t="n">
+        <v>-0.02048120833933353</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-0.1409636288881302</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.9819963574409485</v>
+      </c>
+      <c r="V9" t="b">
+        <v>1</v>
+      </c>
+      <c r="W9" t="b">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ns-8</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>19.762033</v>
+      </c>
+      <c r="C10" t="n">
+        <v>85.70370699999999</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>greenveg</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2020-09-08</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Off Puri</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Puri beach</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="b">
+        <v>0</v>
+      </c>
+      <c r="W10" t="b">
+        <v>0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ns-9</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-23.855629</v>
+      </c>
+      <c r="C11" t="n">
+        <v>35.553179</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>whitewater</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2020-01-02</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Off Tofo Beach</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Mozambique</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>3402.97021484375</v>
+      </c>
+      <c r="K11" t="n">
+        <v>3639.940185546875</v>
+      </c>
+      <c r="L11" t="n">
+        <v>3106.126953125</v>
+      </c>
+      <c r="M11" t="n">
+        <v>2011.216430664062</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1897.858154296875</v>
+      </c>
+      <c r="O11" t="n">
+        <v>814.380615234375</v>
+      </c>
+      <c r="P11" t="n">
+        <v>638.2388305664062</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-17.38692283630371</v>
+      </c>
+      <c r="R11" t="n">
+        <v>-27.10249137878418</v>
+      </c>
+      <c r="S11" t="n">
+        <v>-0.1290073245763779</v>
+      </c>
+      <c r="T11" t="n">
+        <v>-0.1594504415988922</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.2967122495174408</v>
+      </c>
+      <c r="V11" t="b">
+        <v>1</v>
+      </c>
+      <c r="W11" t="b">
+        <v>1</v>
+      </c>
+      <c r="X11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ns-10</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-23.87458</v>
+      </c>
+      <c r="C12" t="n">
+        <v>35.552519</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>whitewater</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2020-01-02</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Off Tofo Beach</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Mozambique</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>3870.646728515625</v>
+      </c>
+      <c r="K12" t="n">
+        <v>4020.180419921875</v>
+      </c>
+      <c r="L12" t="n">
+        <v>3250.481201171875</v>
+      </c>
+      <c r="M12" t="n">
+        <v>2067.744384765625</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1858.496215820312</v>
+      </c>
+      <c r="O12" t="n">
+        <v>878.1804809570312</v>
+      </c>
+      <c r="P12" t="n">
+        <v>698.556396484375</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-18.13891220092773</v>
+      </c>
+      <c r="R12" t="n">
+        <v>-28.37503814697266</v>
+      </c>
+      <c r="S12" t="n">
+        <v>-0.1387260556221008</v>
+      </c>
+      <c r="T12" t="n">
+        <v>-0.1743660271167755</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.32413250207901</v>
+      </c>
+      <c r="V12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W12" t="b">
+        <v>1</v>
+      </c>
+      <c r="X12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ns-11</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>41.384034</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-124.079459</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2022-08-12</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Off northern california</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>205.9477081298828</v>
+      </c>
+      <c r="K13" t="n">
+        <v>157.8758239746094</v>
+      </c>
+      <c r="L13" t="n">
+        <v>29.01960754394531</v>
+      </c>
+      <c r="M13" t="n">
+        <v>17.13725471496582</v>
+      </c>
+      <c r="N13" t="n">
+        <v>23.03921508789062</v>
+      </c>
+      <c r="O13" t="n">
+        <v>23.86274528503418</v>
+      </c>
+      <c r="P13" t="n">
+        <v>27.81045722961426</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>-24.38109588623047</v>
+      </c>
+      <c r="R13" t="n">
+        <v>-28.10061073303223</v>
+      </c>
+      <c r="S13" t="n">
+        <v>-0.3805686831474304</v>
+      </c>
+      <c r="T13" t="n">
+        <v>-0.6200817823410034</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.8050806522369385</v>
+      </c>
+      <c r="V13" t="b">
+        <v>1</v>
+      </c>
+      <c r="W13" t="b">
+        <v>0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ns-12</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>39.655675</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-9.071059999999999</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>whitewater</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2022-10-01</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Off Nazare</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="n">
+        <v>3516.07666015625</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3676.014892578125</v>
+      </c>
+      <c r="L14" t="n">
+        <v>3149.945556640625</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2106.061767578125</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1920.660888671875</v>
+      </c>
+      <c r="O14" t="n">
+        <v>355.0024719238281</v>
+      </c>
+      <c r="P14" t="n">
+        <v>194.9232635498047</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>-14.80997085571289</v>
+      </c>
+      <c r="R14" t="n">
+        <v>-25.25973510742188</v>
+      </c>
+      <c r="S14" t="n">
+        <v>-0.1801728308200836</v>
+      </c>
+      <c r="T14" t="n">
+        <v>-0.2321026474237442</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.2723741233348846</v>
+      </c>
+      <c r="V14" t="b">
+        <v>1</v>
+      </c>
+      <c r="W14" t="b">
+        <v>1</v>
+      </c>
+      <c r="X14" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ns-13</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>39.644781</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-9.066697</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>greenveg</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2022-10-01</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Off Nazare</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>186.3812103271484</v>
+      </c>
+      <c r="K15" t="n">
+        <v>395.0138244628906</v>
+      </c>
+      <c r="L15" t="n">
+        <v>329.6325988769531</v>
+      </c>
+      <c r="M15" t="n">
+        <v>2075.486083984375</v>
+      </c>
+      <c r="N15" t="n">
+        <v>2204.917236328125</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1175.541381835938</v>
+      </c>
+      <c r="P15" t="n">
+        <v>645.9447631835938</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>-13.04985523223877</v>
+      </c>
+      <c r="R15" t="n">
+        <v>-17.47790336608887</v>
+      </c>
+      <c r="S15" t="n">
+        <v>-0.3570275604724884</v>
+      </c>
+      <c r="T15" t="n">
+        <v>-0.2040146738290787</v>
+      </c>
+      <c r="U15" t="n">
+        <v>-0.6804361939430237</v>
+      </c>
+      <c r="V15" t="b">
+        <v>1</v>
+      </c>
+      <c r="W15" t="b">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ns-14</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>25.203775</v>
+      </c>
+      <c r="C16" t="n">
+        <v>55.265823</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>bare</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2022-09-27</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>UAE</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="n">
+        <v>4461.40185546875</v>
+      </c>
+      <c r="K16" t="n">
+        <v>4705.91455078125</v>
+      </c>
+      <c r="L16" t="n">
+        <v>4819.248046875</v>
+      </c>
+      <c r="M16" t="n">
+        <v>4500.0341796875</v>
+      </c>
+      <c r="N16" t="n">
+        <v>4482.341796875</v>
+      </c>
+      <c r="O16" t="n">
+        <v>5569.36767578125</v>
+      </c>
+      <c r="P16" t="n">
+        <v>5400.60693359375</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>-3.858842611312866</v>
+      </c>
+      <c r="R16" t="n">
+        <v>-10.00305461883545</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.05226637795567513</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.07314693927764893</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.02225241810083389</v>
+      </c>
+      <c r="V16" t="b">
+        <v>1</v>
+      </c>
+      <c r="W16" t="b">
+        <v>0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ns-15</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>25.181168</v>
+      </c>
+      <c r="C17" t="n">
+        <v>55.198074</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2022-09-27</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>UAE</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>678.8302001953125</v>
+      </c>
+      <c r="K17" t="n">
+        <v>690.4339599609375</v>
+      </c>
+      <c r="L17" t="n">
+        <v>338.5220031738281</v>
+      </c>
+      <c r="M17" t="n">
+        <v>248.6666717529297</v>
+      </c>
+      <c r="N17" t="n">
+        <v>244.9245300292969</v>
+      </c>
+      <c r="O17" t="n">
+        <v>223.3710632324219</v>
+      </c>
+      <c r="P17" t="n">
+        <v>200.3081817626953</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>-19.6241455078125</v>
+      </c>
+      <c r="R17" t="n">
+        <v>-26.04843902587891</v>
+      </c>
+      <c r="S17" t="n">
+        <v>-0.1801840513944626</v>
+      </c>
+      <c r="T17" t="n">
+        <v>-0.2454206049442291</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.4704325199127197</v>
+      </c>
+      <c r="V17" t="b">
+        <v>1</v>
+      </c>
+      <c r="W17" t="b">
+        <v>0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ns-16</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>21.961674</v>
+      </c>
+      <c r="C18" t="n">
+        <v>89.18479600000001</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>greenveg</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2021-10-31</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Sundarbans</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Bangladesh</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>280.8697814941406</v>
+      </c>
+      <c r="K18" t="n">
+        <v>555.2604370117188</v>
+      </c>
+      <c r="L18" t="n">
+        <v>296.269775390625</v>
+      </c>
+      <c r="M18" t="n">
+        <v>2812.306884765625</v>
+      </c>
+      <c r="N18" t="n">
+        <v>3003.4697265625</v>
+      </c>
+      <c r="O18" t="n">
+        <v>892.9488525390625</v>
+      </c>
+      <c r="P18" t="n">
+        <v>388.181396484375</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>-8.296245574951172</v>
+      </c>
+      <c r="R18" t="n">
+        <v>-14.0239725112915</v>
+      </c>
+      <c r="S18" t="n">
+        <v>-0.5556021332740784</v>
+      </c>
+      <c r="T18" t="n">
+        <v>-0.4442262053489685</v>
+      </c>
+      <c r="U18" t="n">
+        <v>-0.6695176362991333</v>
+      </c>
+      <c r="V18" t="b">
+        <v>1</v>
+      </c>
+      <c r="W18" t="b">
+        <v>0</v>
+      </c>
+      <c r="X18" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ns-17</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>21.969749</v>
+      </c>
+      <c r="C19" t="n">
+        <v>89.178629</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2021-10-31</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Sundarbans</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Bangladesh</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Water is sediment filled</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>870.122802734375</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1095.929809570312</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1060.596435546875</v>
+      </c>
+      <c r="M19" t="n">
+        <v>970.8070068359375</v>
+      </c>
+      <c r="N19" t="n">
+        <v>952.868408203125</v>
+      </c>
+      <c r="O19" t="n">
+        <v>289.3070068359375</v>
+      </c>
+      <c r="P19" t="n">
+        <v>160.9122772216797</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>-18.20453453063965</v>
+      </c>
+      <c r="R19" t="n">
+        <v>-24.62449264526367</v>
+      </c>
+      <c r="S19" t="n">
+        <v>-0.1487147957086563</v>
+      </c>
+      <c r="T19" t="n">
+        <v>-0.1530621647834778</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.06592879444360733</v>
+      </c>
+      <c r="V19" t="b">
+        <v>1</v>
+      </c>
+      <c r="W19" t="b">
+        <v>0</v>
+      </c>
+      <c r="X19" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ns-18</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>9.978316</v>
+      </c>
+      <c r="C20" t="n">
+        <v>76.252207</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>bare</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2022-12-11</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Cochin Docks</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Kerala</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>1358.0830078125</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1590.857177734375</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1731.25341796875</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1777.8525390625</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1843.774169921875</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1959.027709960938</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1801.608276367188</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>-7.064449310302734</v>
+      </c>
+      <c r="R20" t="n">
+        <v>-13.41982364654541</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.04816524311900139</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.08121186494827271</v>
+      </c>
+      <c r="U20" t="n">
+        <v>-0.05485120043158531</v>
+      </c>
+      <c r="V20" t="b">
+        <v>1</v>
+      </c>
+      <c r="W20" t="b">
+        <v>0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ns-19</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>9.975609</v>
+      </c>
+      <c r="C21" t="n">
+        <v>76.25523099999999</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2022-12-11</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Cochin Bay</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Kerala</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>489.859375</v>
+      </c>
+      <c r="K21" t="n">
+        <v>571.3125</v>
+      </c>
+      <c r="L21" t="n">
+        <v>380.609375</v>
+      </c>
+      <c r="M21" t="n">
+        <v>138.546875</v>
+      </c>
+      <c r="N21" t="n">
+        <v>121.046875</v>
+      </c>
+      <c r="O21" t="n">
+        <v>60.65625</v>
+      </c>
+      <c r="P21" t="n">
+        <v>42.90625</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>-20.24484252929688</v>
+      </c>
+      <c r="R21" t="n">
+        <v>-28.2679443359375</v>
+      </c>
+      <c r="S21" t="n">
+        <v>-0.1261710375547409</v>
+      </c>
+      <c r="T21" t="n">
+        <v>-0.1748980730772018</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0.6097844243049622</v>
+      </c>
+      <c r="V21" t="b">
+        <v>1</v>
+      </c>
+      <c r="W21" t="b">
+        <v>0</v>
+      </c>
+      <c r="X21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ns-20</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>41.019946</v>
+      </c>
+      <c r="C22" t="n">
+        <v>28.97316</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>bare</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2021-12-11</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Instanbul bridge</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Turkey</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="n">
+        <v>745.9265747070312</v>
+      </c>
+      <c r="K22" t="n">
+        <v>743.2937622070312</v>
+      </c>
+      <c r="L22" t="n">
+        <v>780.8079223632812</v>
+      </c>
+      <c r="M22" t="n">
+        <v>795.4067993164062</v>
+      </c>
+      <c r="N22" t="n">
+        <v>751.2655639648438</v>
+      </c>
+      <c r="O22" t="n">
+        <v>697.5819091796875</v>
+      </c>
+      <c r="P22" t="n">
+        <v>659.0791015625</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>-2.869668245315552</v>
+      </c>
+      <c r="R22" t="n">
+        <v>-12.56972694396973</v>
+      </c>
+      <c r="S22" t="n">
+        <v>-0.02557701431214809</v>
+      </c>
+      <c r="T22" t="n">
+        <v>-0.01899614185094833</v>
+      </c>
+      <c r="U22" t="n">
+        <v>-0.03210922703146935</v>
+      </c>
+      <c r="V22" t="b">
+        <v>1</v>
+      </c>
+      <c r="W22" t="b">
+        <v>0</v>
+      </c>
+      <c r="X22" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ns-21</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>40.396227</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-111.647693</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2022-05-24</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Snow above Sundance</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="n">
+        <v>8352.8310546875</v>
+      </c>
+      <c r="K23" t="n">
+        <v>8560.779296875</v>
+      </c>
+      <c r="L23" t="n">
+        <v>8638.701171875</v>
+      </c>
+      <c r="M23" t="n">
+        <v>7536.3115234375</v>
+      </c>
+      <c r="N23" t="n">
+        <v>7290.41552734375</v>
+      </c>
+      <c r="O23" t="n">
+        <v>195.3571472167969</v>
+      </c>
+      <c r="P23" t="n">
+        <v>183.2922058105469</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>-18.14537620544434</v>
+      </c>
+      <c r="R23" t="n">
+        <v>-24.11510276794434</v>
+      </c>
+      <c r="S23" t="n">
+        <v>-0.2124138027429581</v>
+      </c>
+      <c r="T23" t="n">
+        <v>-0.2853720784187317</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0.06363208591938019</v>
+      </c>
+      <c r="V23" t="b">
+        <v>1</v>
+      </c>
+      <c r="W23" t="b">
+        <v>0</v>
+      </c>
+      <c r="X23" t="n">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added some samples from Marchetti
</commit_message>
<xml_diff>
--- a/data/labels/gt-bands.xlsx
+++ b/data/labels/gt-bands.xlsx
@@ -14,6 +14,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nonsand" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="florida-fwc" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="wilkerson" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="marchetti" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -21363,24 +21364,11 @@
       <c r="I2" t="n">
         <v>0.31</v>
       </c>
-      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>Mekong River at Wat Sop (No: 00248; p. 71)</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
       <c r="X2" t="b">
         <v>0</v>
       </c>
@@ -21431,7 +21419,6 @@
       <c r="I3" t="n">
         <v>0.18</v>
       </c>
-      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
           <t>Indus (at Hajipur) Pakistan</t>
@@ -21523,7 +21510,6 @@
       <c r="I4" t="n">
         <v>0.45</v>
       </c>
-      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
           <t>Niger River at Jebba, Nigeria (p. 72)</t>
@@ -21615,7 +21601,6 @@
       <c r="I5" t="n">
         <v>0.18</v>
       </c>
-      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
           <t>Yamuna (at Hamirpur, U.P. state) India</t>
@@ -21707,7 +21692,6 @@
       <c r="I6" t="n">
         <v>0.43</v>
       </c>
-      <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
           <t>Ganga (at Mokameh in Bihar state) India</t>
@@ -21799,7 +21783,6 @@
       <c r="I7" t="n">
         <v>0.17</v>
       </c>
-      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>Sutlej (in Samasatta below railway bridge) Pakistan</t>
@@ -21891,7 +21874,6 @@
       <c r="I8" t="n">
         <v>0.04</v>
       </c>
-      <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
           <t>Bennihalli (above Railway Bridge, Gadag Hubli line) India</t>
@@ -22034,6 +22016,748 @@
         <v>1</v>
       </c>
       <c r="Z9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Latitude</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Longitude</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>Site</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="I1" s="5" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="J1" s="5" t="inlineStr">
+        <is>
+          <t>D50</t>
+        </is>
+      </c>
+      <c r="K1" s="5" t="inlineStr">
+        <is>
+          <t>D84</t>
+        </is>
+      </c>
+      <c r="L1" s="5" t="inlineStr">
+        <is>
+          <t>Classification choices</t>
+        </is>
+      </c>
+      <c r="M1" s="5" t="inlineStr">
+        <is>
+          <t>B2_mean</t>
+        </is>
+      </c>
+      <c r="N1" s="5" t="inlineStr">
+        <is>
+          <t>B3_mean</t>
+        </is>
+      </c>
+      <c r="O1" s="5" t="inlineStr">
+        <is>
+          <t>B4_mean</t>
+        </is>
+      </c>
+      <c r="P1" s="5" t="inlineStr">
+        <is>
+          <t>B8_mean</t>
+        </is>
+      </c>
+      <c r="Q1" s="5" t="inlineStr">
+        <is>
+          <t>B8A_mean</t>
+        </is>
+      </c>
+      <c r="R1" s="5" t="inlineStr">
+        <is>
+          <t>B11_mean</t>
+        </is>
+      </c>
+      <c r="S1" s="5" t="inlineStr">
+        <is>
+          <t>B12_mean</t>
+        </is>
+      </c>
+      <c r="T1" s="5" t="inlineStr">
+        <is>
+          <t>VV_mean</t>
+        </is>
+      </c>
+      <c r="U1" s="5" t="inlineStr">
+        <is>
+          <t>VH_mean</t>
+        </is>
+      </c>
+      <c r="V1" s="5" t="inlineStr">
+        <is>
+          <t>mTGSI_mean</t>
+        </is>
+      </c>
+      <c r="W1" s="5" t="inlineStr">
+        <is>
+          <t>BSI_mean</t>
+        </is>
+      </c>
+      <c r="X1" s="5" t="inlineStr">
+        <is>
+          <t>NDWI_mean</t>
+        </is>
+      </c>
+      <c r="Y1" s="5" t="inlineStr">
+        <is>
+          <t>keep</t>
+        </is>
+      </c>
+      <c r="Z1" s="5" t="inlineStr">
+        <is>
+          <t>location_tweaked</t>
+        </is>
+      </c>
+      <c r="AA1" s="5" t="inlineStr">
+        <is>
+          <t>class_code</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>mar-0</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>45.509204</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8.402438999999999</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2018-09-21</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/esp.5394</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>42.4</v>
+      </c>
+      <c r="K2" t="n">
+        <v>88</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>GRID definitions for gravel</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>1862.738891601562</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2232.187255859375</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2427.595947265625</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2450.43359375</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>2447.06396484375</v>
+      </c>
+      <c r="R2" t="n">
+        <v>2708.29052734375</v>
+      </c>
+      <c r="S2" t="n">
+        <v>2362.739013671875</v>
+      </c>
+      <c r="T2" t="n">
+        <v>-7.518976211547852</v>
+      </c>
+      <c r="U2" t="n">
+        <v>-15.48646259307861</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.04200949147343636</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.08687812089920044</v>
+      </c>
+      <c r="X2" t="n">
+        <v>-0.04666387662291527</v>
+      </c>
+      <c r="Y2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>mar-1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>45.059032</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8.900689</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2018-09-20</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/esp.5394</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>34.9</v>
+      </c>
+      <c r="K3" t="n">
+        <v>49</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>GRID definitions for gravel</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>1992.2763671875</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2536.71533203125</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2790.71533203125</v>
+      </c>
+      <c r="P3" t="n">
+        <v>3075.447265625</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>3152.495849609375</v>
+      </c>
+      <c r="R3" t="n">
+        <v>3692.479736328125</v>
+      </c>
+      <c r="S3" t="n">
+        <v>3246.41455078125</v>
+      </c>
+      <c r="T3" t="n">
+        <v>-10.74073505401611</v>
+      </c>
+      <c r="U3" t="n">
+        <v>-18.99478530883789</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.07118057459592819</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.1226525530219078</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-0.09575051814317703</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>mar-2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>45.130529</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9.973807000000001</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>sand</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2018-09-20</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/esp.5394</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>2530.338134765625</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2967.408447265625</v>
+      </c>
+      <c r="O4" t="n">
+        <v>3205.690185546875</v>
+      </c>
+      <c r="P4" t="n">
+        <v>3455.943603515625</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>3506.155029296875</v>
+      </c>
+      <c r="R4" t="n">
+        <v>3926.01416015625</v>
+      </c>
+      <c r="S4" t="n">
+        <v>3619.45068359375</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-11.23505687713623</v>
+      </c>
+      <c r="U4" t="n">
+        <v>-21.05694961547852</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.0535949170589447</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.08782865107059479</v>
+      </c>
+      <c r="X4" t="n">
+        <v>-0.07581157237291336</v>
+      </c>
+      <c r="Y4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>mar-3</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>45.002953</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10.285669</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sand</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2018-09-20</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/esp.5394</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>2083.9775390625</v>
+      </c>
+      <c r="N5" t="n">
+        <v>2484.0224609375</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2703.01123046875</v>
+      </c>
+      <c r="P5" t="n">
+        <v>2892.10107421875</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2878.224609375</v>
+      </c>
+      <c r="R5" t="n">
+        <v>3490.91015625</v>
+      </c>
+      <c r="S5" t="n">
+        <v>3325.44384765625</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-12.91854953765869</v>
+      </c>
+      <c r="U5" t="n">
+        <v>-21.58412742614746</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.07771029323339462</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.1086732149124146</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-0.07581464946269989</v>
+      </c>
+      <c r="Y5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mar-4</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>38.136695</v>
+      </c>
+      <c r="C6" t="n">
+        <v>16.066178</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2018-10-23</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/esp.5394</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>32.8</v>
+      </c>
+      <c r="K6" t="n">
+        <v>71</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>GRID definitions for gravel</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>1883.678588867188</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2170.96435546875</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2251.990966796875</v>
+      </c>
+      <c r="P6" t="n">
+        <v>2226.0625</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2256.115966796875</v>
+      </c>
+      <c r="R6" t="n">
+        <v>2814.084716796875</v>
+      </c>
+      <c r="S6" t="n">
+        <v>2491.321533203125</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-8.212271690368652</v>
+      </c>
+      <c r="U6" t="n">
+        <v>-18.05460357666016</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.05747773498296738</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.1042279452085495</v>
+      </c>
+      <c r="X6" t="n">
+        <v>-0.01253444422036409</v>
+      </c>
+      <c r="Y6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>mar-5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>38.126562</v>
+      </c>
+      <c r="C7" t="n">
+        <v>16.141612</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>gravel</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2018-10-24</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>fluvial</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/esp.5394</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>42.3</v>
+      </c>
+      <c r="K7" t="n">
+        <v>69</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>GRID definitions for gravel</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>1964.852905273438</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2262.558837890625</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2412.441162109375</v>
+      </c>
+      <c r="P7" t="n">
+        <v>2509</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2632.588134765625</v>
+      </c>
+      <c r="R7" t="n">
+        <v>3132.411865234375</v>
+      </c>
+      <c r="S7" t="n">
+        <v>2756.470703125</v>
+      </c>
+      <c r="T7" t="n">
+        <v>-10.61365032196045</v>
+      </c>
+      <c r="U7" t="n">
+        <v>-19.78536415100098</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.05866438150405884</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.1072599068284035</v>
+      </c>
+      <c r="X7" t="n">
+        <v>-0.05146156251430511</v>
+      </c>
+      <c r="Y7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>